<commit_message>
Added General Solver Function and Intermediary Transaction Creation
</commit_message>
<xml_diff>
--- a/SpartanTrader10/SpartanTrader10.xlsx
+++ b/SpartanTrader10/SpartanTrader10.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
   <si>
     <t>Stock Market</t>
   </si>
@@ -249,6 +249,27 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>W*Delta</t>
+  </si>
+  <si>
+    <t>W*Gamma</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -496,14 +517,14 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -514,23 +535,23 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1121,11 +1142,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$AV$4</c:f>
+              <c:f>Dashboard!$AS$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1144,10 +1165,31 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$AV$5:$AV$11</c:f>
+              <c:f>Dashboard!$AS$5:$AS$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1158,11 +1200,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$AW$4</c:f>
+              <c:f>Dashboard!$AT$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1181,10 +1223,31 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$AW$5:$AW$11</c:f>
+              <c:f>Dashboard!$AT$5:$AT$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1195,11 +1258,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$AX$4</c:f>
+              <c:f>Dashboard!$AU$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1218,10 +1281,31 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$AX$5:$AX$11</c:f>
+              <c:f>Dashboard!$AU$5:$AU$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1232,11 +1316,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$AY$4</c:f>
+              <c:f>Dashboard!#REF!</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column4</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1255,10 +1339,13 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$AY$5:$AY$11</c:f>
+              <c:f>Dashboard!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1273,11 +1360,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="421373240"/>
-        <c:axId val="421369712"/>
+        <c:axId val="418214960"/>
+        <c:axId val="418212216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421373240"/>
+        <c:axId val="418214960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421369712"/>
+        <c:crossAx val="418212216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421369712"/>
+        <c:axId val="418212216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,7 +1465,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421373240"/>
+        <c:crossAx val="418214960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1644,11 +1731,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="423037936"/>
-        <c:axId val="423035976"/>
+        <c:axId val="420314808"/>
+        <c:axId val="420311672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="423037936"/>
+        <c:axId val="420314808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1690,7 +1777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423035976"/>
+        <c:crossAx val="420311672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1698,7 +1785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423035976"/>
+        <c:axId val="420311672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,7 +1836,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423037936"/>
+        <c:crossAx val="420314808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2058,11 +2145,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="423038328"/>
-        <c:axId val="423035584"/>
+        <c:axId val="420310888"/>
+        <c:axId val="420315200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="423038328"/>
+        <c:axId val="420310888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2104,7 +2191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423035584"/>
+        <c:crossAx val="420315200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2112,7 +2199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423035584"/>
+        <c:axId val="420315200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,7 +2250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423038328"/>
+        <c:crossAx val="420310888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5153,8 +5240,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="TELO" displayName="TELO" ref="AV4:AY11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="AV4:AY11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="TELO" displayName="TELO" ref="AX2:BA9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="AX2:BA9"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column1" dataDxfId="13"/>
     <tableColumn id="2" name="Column2" dataDxfId="12"/>
@@ -5552,10 +5639,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AY34"/>
+  <dimension ref="A1:BA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="AH31" workbookViewId="0">
+      <selection activeCell="AR35" sqref="AR35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5572,40 +5659,42 @@
     <col min="11" max="11" width="17.140625" style="5" customWidth="1"/>
     <col min="12" max="16" width="8.7109375" style="5"/>
     <col min="17" max="21" width="10.28515625" style="5" customWidth="1"/>
-    <col min="22" max="47" width="8.7109375" style="5"/>
+    <col min="22" max="38" width="8.7109375" style="5"/>
+    <col min="39" max="45" width="11" style="5" customWidth="1"/>
+    <col min="46" max="47" width="8.7109375" style="5"/>
     <col min="48" max="51" width="11" style="5" customWidth="1"/>
     <col min="52" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:53" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
-    <row r="2" spans="1:51" ht="26.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:53" ht="26.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="I2" s="23" t="s">
         <v>51</v>
       </c>
@@ -5640,14 +5729,53 @@
       </c>
       <c r="W2" s="35"/>
       <c r="X2" s="35"/>
+      <c r="AM2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR2" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU2" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA2" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:51" ht="9.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+    <row r="3" spans="1:53" ht="9.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="9"/>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
@@ -5666,7 +5794,7 @@
       <c r="W3" s="35"/>
       <c r="X3" s="35"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>41</v>
       </c>
@@ -5702,20 +5830,26 @@
       <c r="O4" s="29">
         <v>0</v>
       </c>
-      <c r="AV4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AY4" s="5" t="s">
-        <v>4</v>
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="25"/>
+      <c r="AR4" s="25"/>
+      <c r="AS4" s="25">
+        <f>AQ4*AN4</f>
+        <v>0</v>
+      </c>
+      <c r="AT4" s="25">
+        <f>AQ4*AO4</f>
+        <v>0</v>
+      </c>
+      <c r="AU4" s="25">
+        <f>AP4*AQ4</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -5749,8 +5883,26 @@
       <c r="O5" s="29">
         <v>0</v>
       </c>
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="25"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="25"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25">
+        <f t="shared" ref="AS5:AS35" si="0">AQ5*AN5</f>
+        <v>0</v>
+      </c>
+      <c r="AT5" s="25">
+        <f t="shared" ref="AT5:AT35" si="1">AQ5*AO5</f>
+        <v>0</v>
+      </c>
+      <c r="AU5" s="25">
+        <f t="shared" ref="AU5:AU35" si="2">AP5*AQ5</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>43</v>
       </c>
@@ -5784,8 +5936,26 @@
       <c r="O6" s="29">
         <v>0</v>
       </c>
+      <c r="AM6" s="25"/>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="25"/>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT6" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU6" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="C7" s="10"/>
       <c r="E7" s="8" t="s">
@@ -5815,8 +5985,26 @@
       <c r="O7" s="29">
         <v>0</v>
       </c>
+      <c r="AM7" s="25"/>
+      <c r="AN7" s="25"/>
+      <c r="AO7" s="25"/>
+      <c r="AP7" s="25"/>
+      <c r="AQ7" s="25"/>
+      <c r="AR7" s="25"/>
+      <c r="AS7" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT7" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU7" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>44</v>
       </c>
@@ -5846,8 +6034,26 @@
       <c r="O8" s="29">
         <v>0</v>
       </c>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="25"/>
+      <c r="AO8" s="25"/>
+      <c r="AP8" s="25"/>
+      <c r="AQ8" s="25"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT8" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>45</v>
       </c>
@@ -5881,8 +6087,26 @@
       <c r="O9" s="29">
         <v>0</v>
       </c>
+      <c r="AM9" s="25"/>
+      <c r="AN9" s="25"/>
+      <c r="AO9" s="25"/>
+      <c r="AP9" s="25"/>
+      <c r="AQ9" s="25"/>
+      <c r="AR9" s="25"/>
+      <c r="AS9" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT9" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
@@ -5916,8 +6140,26 @@
       <c r="O10" s="29">
         <v>0</v>
       </c>
+      <c r="AM10" s="25"/>
+      <c r="AN10" s="25"/>
+      <c r="AO10" s="25"/>
+      <c r="AP10" s="25"/>
+      <c r="AQ10" s="25"/>
+      <c r="AR10" s="25"/>
+      <c r="AS10" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT10" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="15"/>
@@ -5948,8 +6190,26 @@
       <c r="O11" s="29">
         <v>0</v>
       </c>
+      <c r="AM11" s="25"/>
+      <c r="AN11" s="25"/>
+      <c r="AO11" s="25"/>
+      <c r="AP11" s="25"/>
+      <c r="AQ11" s="25"/>
+      <c r="AR11" s="25"/>
+      <c r="AS11" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT11" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU11" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
@@ -5983,8 +6243,26 @@
       <c r="O12" s="29">
         <v>0</v>
       </c>
+      <c r="AM12" s="25"/>
+      <c r="AN12" s="25"/>
+      <c r="AO12" s="25"/>
+      <c r="AP12" s="25"/>
+      <c r="AQ12" s="25"/>
+      <c r="AR12" s="25"/>
+      <c r="AS12" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT12" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU12" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>47</v>
       </c>
@@ -6018,8 +6296,26 @@
       <c r="O13" s="29">
         <v>0</v>
       </c>
+      <c r="AM13" s="25"/>
+      <c r="AN13" s="25"/>
+      <c r="AO13" s="25"/>
+      <c r="AP13" s="25"/>
+      <c r="AQ13" s="25"/>
+      <c r="AR13" s="25"/>
+      <c r="AS13" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT13" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
@@ -6049,8 +6345,26 @@
       <c r="O14" s="29">
         <v>0</v>
       </c>
+      <c r="AM14" s="25"/>
+      <c r="AN14" s="25"/>
+      <c r="AO14" s="25"/>
+      <c r="AP14" s="25"/>
+      <c r="AQ14" s="25"/>
+      <c r="AR14" s="25"/>
+      <c r="AS14" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT14" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="C15" s="10"/>
       <c r="E15" s="8" t="s">
@@ -6080,8 +6394,26 @@
       <c r="O15" s="29">
         <v>0</v>
       </c>
+      <c r="AM15" s="25"/>
+      <c r="AN15" s="25"/>
+      <c r="AO15" s="25"/>
+      <c r="AP15" s="25"/>
+      <c r="AQ15" s="25"/>
+      <c r="AR15" s="25"/>
+      <c r="AS15" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT15" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU15" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
@@ -6101,8 +6433,26 @@
       <c r="M16" s="25"/>
       <c r="N16" s="25"/>
       <c r="O16" s="25"/>
+      <c r="AM16" s="25"/>
+      <c r="AN16" s="25"/>
+      <c r="AO16" s="25"/>
+      <c r="AP16" s="25"/>
+      <c r="AQ16" s="25"/>
+      <c r="AR16" s="25"/>
+      <c r="AS16" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT16" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU16" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
@@ -6122,8 +6472,26 @@
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
+      <c r="AM17" s="25"/>
+      <c r="AN17" s="25"/>
+      <c r="AO17" s="25"/>
+      <c r="AP17" s="25"/>
+      <c r="AQ17" s="25"/>
+      <c r="AR17" s="25"/>
+      <c r="AS17" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT17" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU17" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>48</v>
       </c>
@@ -6137,8 +6505,26 @@
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
       <c r="O18" s="25"/>
+      <c r="AM18" s="25"/>
+      <c r="AN18" s="25"/>
+      <c r="AO18" s="25"/>
+      <c r="AP18" s="25"/>
+      <c r="AQ18" s="25"/>
+      <c r="AR18" s="25"/>
+      <c r="AS18" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT18" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU18" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>40</v>
       </c>
@@ -6155,8 +6541,26 @@
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
+      <c r="AM19" s="25"/>
+      <c r="AN19" s="25"/>
+      <c r="AO19" s="25"/>
+      <c r="AP19" s="25"/>
+      <c r="AQ19" s="25"/>
+      <c r="AR19" s="25"/>
+      <c r="AS19" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT19" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU19" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -6171,12 +6575,30 @@
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
+      <c r="AM20" s="25"/>
+      <c r="AN20" s="25"/>
+      <c r="AO20" s="25"/>
+      <c r="AP20" s="25"/>
+      <c r="AQ20" s="25"/>
+      <c r="AR20" s="25"/>
+      <c r="AS20" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT20" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU20" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="39" t="s">
+    <row r="21" spans="1:47" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="40"/>
+      <c r="G21" s="31"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
@@ -6184,10 +6606,28 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
+      <c r="AM21" s="25"/>
+      <c r="AN21" s="25"/>
+      <c r="AO21" s="25"/>
+      <c r="AP21" s="25"/>
+      <c r="AQ21" s="25"/>
+      <c r="AR21" s="25"/>
+      <c r="AS21" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT21" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU21" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
+    <row r="22" spans="1:47" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
@@ -6195,10 +6635,28 @@
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
+      <c r="AM22" s="25"/>
+      <c r="AN22" s="25"/>
+      <c r="AO22" s="25"/>
+      <c r="AP22" s="25"/>
+      <c r="AQ22" s="25"/>
+      <c r="AR22" s="25"/>
+      <c r="AS22" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT22" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU22" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -6206,10 +6664,28 @@
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
+      <c r="AM23" s="25"/>
+      <c r="AN23" s="25"/>
+      <c r="AO23" s="25"/>
+      <c r="AP23" s="25"/>
+      <c r="AQ23" s="25"/>
+      <c r="AR23" s="25"/>
+      <c r="AS23" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT23" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU23" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
@@ -6217,10 +6693,28 @@
       <c r="M24" s="25"/>
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
+      <c r="AM24" s="25"/>
+      <c r="AN24" s="25"/>
+      <c r="AO24" s="25"/>
+      <c r="AP24" s="25"/>
+      <c r="AQ24" s="25"/>
+      <c r="AR24" s="25"/>
+      <c r="AS24" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT24" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU24" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -6228,10 +6722,28 @@
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
+      <c r="AM25" s="25"/>
+      <c r="AN25" s="25"/>
+      <c r="AO25" s="25"/>
+      <c r="AP25" s="25"/>
+      <c r="AQ25" s="25"/>
+      <c r="AR25" s="25"/>
+      <c r="AS25" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT25" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU25" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -6239,10 +6751,28 @@
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
       <c r="O26" s="25"/>
+      <c r="AM26" s="25"/>
+      <c r="AN26" s="25"/>
+      <c r="AO26" s="25"/>
+      <c r="AP26" s="25"/>
+      <c r="AQ26" s="25"/>
+      <c r="AR26" s="25"/>
+      <c r="AS26" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT26" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU26" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
@@ -6250,8 +6780,26 @@
       <c r="M27" s="25"/>
       <c r="N27" s="25"/>
       <c r="O27" s="25"/>
+      <c r="AM27" s="25"/>
+      <c r="AN27" s="25"/>
+      <c r="AO27" s="25"/>
+      <c r="AP27" s="25"/>
+      <c r="AQ27" s="25"/>
+      <c r="AR27" s="25"/>
+      <c r="AS27" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT27" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU27" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
@@ -6259,8 +6807,26 @@
       <c r="M28" s="25"/>
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
+      <c r="AM28" s="25"/>
+      <c r="AN28" s="25"/>
+      <c r="AO28" s="25"/>
+      <c r="AP28" s="25"/>
+      <c r="AQ28" s="25"/>
+      <c r="AR28" s="25"/>
+      <c r="AS28" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT28" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU28" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="I29" s="25"/>
       <c r="J29" s="25"/>
       <c r="K29" s="25"/>
@@ -6268,8 +6834,26 @@
       <c r="M29" s="25"/>
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
+      <c r="AM29" s="25"/>
+      <c r="AN29" s="25"/>
+      <c r="AO29" s="25"/>
+      <c r="AP29" s="25"/>
+      <c r="AQ29" s="25"/>
+      <c r="AR29" s="25"/>
+      <c r="AS29" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT29" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU29" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="I30" s="25"/>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
@@ -6277,8 +6861,20 @@
       <c r="M30" s="25"/>
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
+      <c r="AS30" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT30" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU30" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
@@ -6286,8 +6882,20 @@
       <c r="M31" s="25"/>
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
+      <c r="AS31" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT31" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU31" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
@@ -6295,8 +6903,20 @@
       <c r="M32" s="25"/>
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
+      <c r="AS32" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT32" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU32" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
@@ -6304,8 +6924,20 @@
       <c r="M33" s="25"/>
       <c r="N33" s="25"/>
       <c r="O33" s="25"/>
+      <c r="AS33" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT33" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU33" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
@@ -6313,18 +6945,44 @@
       <c r="M34" s="25"/>
       <c r="N34" s="25"/>
       <c r="O34" s="25"/>
+      <c r="AS34" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT34" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU34" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="AS35" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT35" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU35" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="8">
-    <mergeCell ref="R2:T3"/>
-    <mergeCell ref="V2:X3"/>
-    <mergeCell ref="E2:G3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="F21:G27"/>
     <mergeCell ref="A19:D19"/>
+    <mergeCell ref="R2:T3"/>
+    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="E2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6832,27 +7490,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="Q1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="Q1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Trader with no bugs working. Supporting functions added. Commented out code to control trading frequency behavior.
</commit_message>
<xml_diff>
--- a/SpartanTrader10/SpartanTrader10.xlsx
+++ b/SpartanTrader10/SpartanTrader10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="7920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -388,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +416,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -517,6 +523,15 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -535,17 +550,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -553,6 +559,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,6 +837,108 @@
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="13A3AB2DF190D214B5019698171B1D64DD8681"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2037"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="11165"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1818A3A8A1BA671426E1B206184EE4BFD9C941"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2963"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="529"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1454BFB5E1D645141091B73211A51887DA7C71"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BBCC80AD153C4144421923510F58B2602C731"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1A18C20641A72C1401B18C5C1A90A56B754661"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="12486F748194FB14E891ADBE158DFF48F524B1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1376"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
@@ -845,7 +954,109 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1C2F7952D1F41C14E781A8601CF9C77B05EF91"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2C443C73C2139424511282E223BA9D59E01A72"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9DF148E8B9C34E949E39BB769715A2AAD5B239"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="794"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="84E0CECCD8B11684AA8882828679A4649A6238"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="475CE45464FC5C44EC1491CD403B214C11B264"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3A737A9013AE31342143AAC332FEB1D70166A3"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -862,216 +1073,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3A737A9013AE31342143AAC332FEB1D70166A3"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="475CE45464FC5C44EC1491CD403B214C11B264"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="84E0CECCD8B11684AA8882828679A4649A6238"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="9DF148E8B9C34E949E39BB769715A2AAD5B239"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="794"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="13A3AB2DF190D214B5019698171B1D64DD8681"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2037"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="6403"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2C443C73C2139424511282E223BA9D59E01A72"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1C2F7952D1F41C14E781A8601CF9C77B05EF91"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="12486F748194FB14E891ADBE158DFF48F524B1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1376"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1A18C20641A72C1401B18C5C1A90A56B754661"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1535"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BBCC80AD153C4144421923510F58B2602C731"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1454BFB5E1D645141091B73211A51887DA7C71"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1818A3A8A1BA671426E1B206184EE4BFD9C941"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2963"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="529"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B41DF30A103CB1433018E231B7416FB5ED861"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B9CFAB0817D4614E371BA261C76ECA0C6DA41"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1105,7 +1112,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B9CFAB0817D4614E371BA261C76ECA0C6DA41"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B41DF30A103CB1433018E231B7416FB5ED861"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1360,11 +1367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="418214960"/>
-        <c:axId val="418212216"/>
+        <c:axId val="424022376"/>
+        <c:axId val="424027472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="418214960"/>
+        <c:axId val="424022376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418212216"/>
+        <c:crossAx val="424027472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1414,7 +1421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418212216"/>
+        <c:axId val="424027472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,7 +1472,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418214960"/>
+        <c:crossAx val="424022376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1731,11 +1738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="420314808"/>
-        <c:axId val="420311672"/>
+        <c:axId val="424024336"/>
+        <c:axId val="424410080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="420314808"/>
+        <c:axId val="424024336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420311672"/>
+        <c:crossAx val="424410080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1785,7 +1792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="420311672"/>
+        <c:axId val="424410080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420314808"/>
+        <c:crossAx val="424024336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2145,11 +2152,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="420310888"/>
-        <c:axId val="420315200"/>
+        <c:axId val="424410472"/>
+        <c:axId val="424409296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="420310888"/>
+        <c:axId val="424410472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2198,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420315200"/>
+        <c:crossAx val="424409296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2199,7 +2206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="420315200"/>
+        <c:axId val="424409296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2250,7 +2257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420310888"/>
+        <c:crossAx val="424410472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4030,7 +4037,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4092,7 +4099,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4154,7 +4161,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4216,7 +4223,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4278,7 +4285,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4340,7 +4347,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4402,7 +4409,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4464,7 +4471,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4526,7 +4533,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4588,7 +4595,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4650,7 +4657,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4712,7 +4719,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4774,7 +4781,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4836,7 +4843,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4879,16 +4886,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>133350</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>16</xdr:col>
-          <xdr:colOff>152400</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>180975</xdr:colOff>
+          <xdr:row>60</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4898,7 +4905,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38AB541D-4CF7-4DDA-B363-D444372BF1B1}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38AB541D-4CF7-4DDA-B363-D444372BF1B1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4995,7 +5002,7 @@
                   <a14:compatExt spid="_x0000_s5121"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001140000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5057,7 +5064,7 @@
                   <a14:compatExt spid="_x0000_s5122"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002140000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5114,7 +5121,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5150,7 +5157,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5639,10 +5646,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:BA35"/>
+  <dimension ref="A1:BA84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH31" workbookViewId="0">
-      <selection activeCell="AR35" sqref="AR35"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5667,34 +5674,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:53" ht="26.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="E2" s="36" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="E2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
       <c r="I2" s="23" t="s">
         <v>51</v>
       </c>
@@ -5718,17 +5725,17 @@
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
       <c r="U2" s="7"/>
-      <c r="V2" s="35" t="s">
+      <c r="V2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
       <c r="AM2" s="25" t="s">
         <v>70</v>
       </c>
@@ -5770,12 +5777,12 @@
       </c>
     </row>
     <row r="3" spans="1:53" ht="9.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="9"/>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
@@ -5786,13 +5793,13 @@
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -6525,12 +6532,12 @@
       </c>
     </row>
     <row r="19" spans="1:47" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -6595,10 +6602,10 @@
       </c>
     </row>
     <row r="21" spans="1:47" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="31"/>
+      <c r="G21" s="34"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
@@ -6626,8 +6633,8 @@
       </c>
     </row>
     <row r="22" spans="1:47" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
@@ -6655,8 +6662,8 @@
       </c>
     </row>
     <row r="23" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -6684,8 +6691,8 @@
       </c>
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
@@ -6713,8 +6720,8 @@
       </c>
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -6742,8 +6749,8 @@
       </c>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -6771,8 +6778,8 @@
       </c>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
@@ -6972,17 +6979,467 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+    </row>
+    <row r="41" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="42"/>
+      <c r="M41" s="42"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="42"/>
+    </row>
+    <row r="42" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+    </row>
+    <row r="43" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+    </row>
+    <row r="44" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="42"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="42"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="42"/>
+    </row>
+    <row r="45" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="42"/>
+    </row>
+    <row r="46" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
+      <c r="N46" s="42"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="42"/>
+    </row>
+    <row r="47" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="42"/>
+      <c r="M47" s="42"/>
+      <c r="N47" s="42"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="42"/>
+    </row>
+    <row r="48" spans="9:47" x14ac:dyDescent="0.25">
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="42"/>
+      <c r="M48" s="42"/>
+      <c r="N48" s="42"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="42"/>
+    </row>
+    <row r="49" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
+      <c r="L49" s="42"/>
+      <c r="M49" s="42"/>
+      <c r="N49" s="42"/>
+      <c r="O49" s="42"/>
+      <c r="P49" s="42"/>
+    </row>
+    <row r="50" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I50" s="42"/>
+      <c r="J50" s="42"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="42"/>
+      <c r="P50" s="42"/>
+    </row>
+    <row r="51" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="42"/>
+      <c r="L51" s="42"/>
+      <c r="M51" s="42"/>
+      <c r="N51" s="42"/>
+      <c r="O51" s="42"/>
+      <c r="P51" s="42"/>
+    </row>
+    <row r="52" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I52" s="42"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="42"/>
+      <c r="P52" s="42"/>
+    </row>
+    <row r="53" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="42"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
+    </row>
+    <row r="54" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="42"/>
+      <c r="N54" s="42"/>
+      <c r="O54" s="42"/>
+      <c r="P54" s="42"/>
+    </row>
+    <row r="55" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I55" s="42"/>
+      <c r="J55" s="42"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+      <c r="M55" s="42"/>
+      <c r="N55" s="42"/>
+      <c r="O55" s="42"/>
+      <c r="P55" s="42"/>
+    </row>
+    <row r="56" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I56" s="42"/>
+      <c r="J56" s="42"/>
+      <c r="K56" s="42"/>
+      <c r="L56" s="42"/>
+      <c r="M56" s="42"/>
+      <c r="N56" s="42"/>
+      <c r="O56" s="42"/>
+      <c r="P56" s="42"/>
+    </row>
+    <row r="57" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I57" s="42"/>
+      <c r="J57" s="42"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="42"/>
+      <c r="N57" s="42"/>
+      <c r="O57" s="42"/>
+      <c r="P57" s="42"/>
+    </row>
+    <row r="58" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I58" s="42"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="42"/>
+      <c r="N58" s="42"/>
+      <c r="O58" s="42"/>
+      <c r="P58" s="42"/>
+    </row>
+    <row r="59" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="42"/>
+      <c r="N59" s="42"/>
+      <c r="O59" s="42"/>
+      <c r="P59" s="42"/>
+    </row>
+    <row r="60" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I60" s="42"/>
+      <c r="J60" s="42"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="42"/>
+      <c r="M60" s="42"/>
+      <c r="N60" s="42"/>
+      <c r="O60" s="42"/>
+      <c r="P60" s="42"/>
+    </row>
+    <row r="61" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I61" s="42"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="42"/>
+      <c r="M61" s="42"/>
+      <c r="N61" s="42"/>
+      <c r="O61" s="42"/>
+      <c r="P61" s="42"/>
+    </row>
+    <row r="62" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I62" s="42"/>
+      <c r="J62" s="42"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="42"/>
+      <c r="M62" s="42"/>
+      <c r="N62" s="42"/>
+      <c r="O62" s="42"/>
+      <c r="P62" s="42"/>
+    </row>
+    <row r="63" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I63" s="42"/>
+      <c r="J63" s="42"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="42"/>
+      <c r="M63" s="42"/>
+      <c r="N63" s="42"/>
+      <c r="O63" s="42"/>
+      <c r="P63" s="42"/>
+    </row>
+    <row r="64" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I64" s="42"/>
+      <c r="J64" s="42"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="42"/>
+      <c r="N64" s="42"/>
+      <c r="O64" s="42"/>
+      <c r="P64" s="42"/>
+    </row>
+    <row r="65" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I65" s="42"/>
+      <c r="J65" s="42"/>
+      <c r="K65" s="42"/>
+      <c r="L65" s="42"/>
+      <c r="M65" s="42"/>
+      <c r="N65" s="42"/>
+      <c r="O65" s="42"/>
+      <c r="P65" s="42"/>
+    </row>
+    <row r="66" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I66" s="42"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="42"/>
+      <c r="M66" s="42"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="42"/>
+      <c r="P66" s="42"/>
+    </row>
+    <row r="67" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I67" s="42"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="42"/>
+      <c r="L67" s="42"/>
+      <c r="M67" s="42"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="42"/>
+      <c r="P67" s="42"/>
+    </row>
+    <row r="68" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I68" s="42"/>
+      <c r="J68" s="42"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="42"/>
+      <c r="M68" s="42"/>
+      <c r="N68" s="42"/>
+      <c r="O68" s="42"/>
+      <c r="P68" s="42"/>
+    </row>
+    <row r="69" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I69" s="42"/>
+      <c r="J69" s="42"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="42"/>
+      <c r="O69" s="42"/>
+      <c r="P69" s="42"/>
+    </row>
+    <row r="70" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I70" s="42"/>
+      <c r="J70" s="42"/>
+      <c r="K70" s="42"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="42"/>
+      <c r="N70" s="42"/>
+      <c r="O70" s="42"/>
+      <c r="P70" s="42"/>
+    </row>
+    <row r="71" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I71" s="42"/>
+      <c r="J71" s="42"/>
+      <c r="K71" s="42"/>
+      <c r="L71" s="42"/>
+      <c r="M71" s="42"/>
+      <c r="N71" s="42"/>
+      <c r="O71" s="42"/>
+      <c r="P71" s="42"/>
+    </row>
+    <row r="72" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I72" s="42"/>
+      <c r="J72" s="42"/>
+      <c r="K72" s="42"/>
+      <c r="L72" s="42"/>
+      <c r="M72" s="42"/>
+      <c r="N72" s="42"/>
+      <c r="O72" s="42"/>
+      <c r="P72" s="42"/>
+    </row>
+    <row r="73" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I73" s="42"/>
+      <c r="J73" s="42"/>
+      <c r="K73" s="42"/>
+      <c r="L73" s="42"/>
+      <c r="M73" s="42"/>
+      <c r="N73" s="42"/>
+      <c r="O73" s="42"/>
+      <c r="P73" s="42"/>
+    </row>
+    <row r="74" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I74" s="42"/>
+      <c r="J74" s="42"/>
+      <c r="K74" s="42"/>
+      <c r="L74" s="42"/>
+      <c r="M74" s="42"/>
+      <c r="N74" s="42"/>
+      <c r="O74" s="42"/>
+      <c r="P74" s="42"/>
+    </row>
+    <row r="75" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I75" s="42"/>
+      <c r="J75" s="42"/>
+      <c r="K75" s="42"/>
+      <c r="L75" s="42"/>
+      <c r="M75" s="42"/>
+      <c r="N75" s="42"/>
+      <c r="O75" s="42"/>
+      <c r="P75" s="42"/>
+    </row>
+    <row r="76" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I76" s="42"/>
+      <c r="J76" s="42"/>
+      <c r="K76" s="42"/>
+      <c r="L76" s="42"/>
+      <c r="M76" s="42"/>
+      <c r="N76" s="42"/>
+      <c r="O76" s="42"/>
+      <c r="P76" s="42"/>
+    </row>
+    <row r="77" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I77" s="42"/>
+      <c r="J77" s="42"/>
+      <c r="K77" s="42"/>
+      <c r="L77" s="42"/>
+      <c r="M77" s="42"/>
+      <c r="N77" s="42"/>
+      <c r="O77" s="42"/>
+      <c r="P77" s="42"/>
+    </row>
+    <row r="78" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I78" s="42"/>
+      <c r="J78" s="42"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="42"/>
+      <c r="M78" s="42"/>
+      <c r="N78" s="42"/>
+      <c r="O78" s="42"/>
+      <c r="P78" s="42"/>
+    </row>
+    <row r="79" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I79" s="42"/>
+      <c r="J79" s="42"/>
+      <c r="K79" s="42"/>
+      <c r="L79" s="42"/>
+      <c r="M79" s="42"/>
+      <c r="N79" s="42"/>
+      <c r="O79" s="42"/>
+      <c r="P79" s="42"/>
+    </row>
+    <row r="80" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I80" s="42"/>
+      <c r="J80" s="42"/>
+      <c r="K80" s="42"/>
+      <c r="L80" s="42"/>
+      <c r="M80" s="42"/>
+      <c r="N80" s="42"/>
+      <c r="O80" s="42"/>
+      <c r="P80" s="42"/>
+    </row>
+    <row r="81" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I81" s="42"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="42"/>
+      <c r="M81" s="42"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="42"/>
+      <c r="P81" s="42"/>
+    </row>
+    <row r="82" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I82" s="42"/>
+      <c r="J82" s="42"/>
+      <c r="K82" s="42"/>
+      <c r="L82" s="42"/>
+      <c r="M82" s="42"/>
+      <c r="N82" s="42"/>
+      <c r="O82" s="42"/>
+      <c r="P82" s="42"/>
+    </row>
+    <row r="83" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I83" s="42"/>
+      <c r="J83" s="42"/>
+      <c r="K83" s="42"/>
+      <c r="L83" s="42"/>
+      <c r="M83" s="42"/>
+      <c r="N83" s="42"/>
+      <c r="O83" s="42"/>
+      <c r="P83" s="42"/>
+    </row>
+    <row r="84" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I84" s="42"/>
+      <c r="J84" s="42"/>
+      <c r="K84" s="42"/>
+      <c r="L84" s="42"/>
+      <c r="M84" s="42"/>
+      <c r="N84" s="42"/>
+      <c r="O84" s="42"/>
+      <c r="P84" s="42"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="8">
+    <mergeCell ref="R2:T3"/>
+    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="E2:G3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="F21:G27"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="R2:T3"/>
-    <mergeCell ref="V2:X3"/>
-    <mergeCell ref="E2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6991,19 +7448,94 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId4" name="_ActiveXWrapper14">
+        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper15">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>17</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>60</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1033" r:id="rId6" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>504825</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId6" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId8" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>209550</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId8" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -7011,163 +7543,88 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId4" name="_ActiveXWrapper14"/>
+        <control shapeId="1028" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId6" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1027" r:id="rId12" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>104775</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>542925</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1040" r:id="rId6" name="_ActiveXWrapper13"/>
+        <control shapeId="1027" r:id="rId12" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId8" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="1026" r:id="rId14" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>590550</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1039" r:id="rId8" name="_ActiveXWrapper12"/>
+        <control shapeId="1026" r:id="rId14" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId10" name="_ActiveXWrapper11">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="1025" r:id="rId16" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId10" name="_ActiveXWrapper11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId12" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1037" r:id="rId12" name="_ActiveXWrapper10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId16" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId16" name="_ActiveXWrapper8"/>
+        <control shapeId="1025" r:id="rId16" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1034" r:id="rId18" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -7191,69 +7648,169 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId19" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+        <control shapeId="1035" r:id="rId20" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId19" name="_ActiveXWrapper1"/>
+        <control shapeId="1035" r:id="rId20" name="_ActiveXWrapper8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId21" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
+        <control shapeId="1036" r:id="rId22" name="_ActiveXWrapper9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>200025</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>590550</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId21" name="_ActiveXWrapper2"/>
+        <control shapeId="1036" r:id="rId22" name="_ActiveXWrapper9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId23" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
+        <control shapeId="1037" r:id="rId24" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>542925</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:colOff>514350</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId24" name="_ActiveXWrapper10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId26" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId26" name="_ActiveXWrapper11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId28" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId29">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId28" name="_ActiveXWrapper12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1040" r:id="rId30" name="_ActiveXWrapper13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1040" r:id="rId30" name="_ActiveXWrapper13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId32" name="_ActiveXWrapper14">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>504825</xdr:colOff>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -7261,107 +7818,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId23" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId25" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId26">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId25" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId27" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId28">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId27" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId29" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId30">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId29" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId31" name="_ActiveXWrapper15">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1042" r:id="rId31" name="_ActiveXWrapper15"/>
+        <control shapeId="1041" r:id="rId32" name="_ActiveXWrapper14"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7419,8 +7876,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="5122" r:id="rId4" name="_ActiveXWrapper2">
+        <control shapeId="5121" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="5121" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="5122" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -7439,32 +7921,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="5122" r:id="rId4" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="5121" r:id="rId6" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="5121" r:id="rId6" name="_ActiveXWrapper1"/>
+        <control shapeId="5122" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
July Options, negative delta bet added
</commit_message>
<xml_diff>
--- a/SpartanTrader10/SpartanTrader10.xlsx
+++ b/SpartanTrader10/SpartanTrader10.xlsx
@@ -523,11 +523,18 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -547,19 +554,12 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,6 +837,108 @@
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1E2A52455132D914AEE1AEF2144BD19AEA9CE1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="6218"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="22AE137DF231F5242212B9B62458710E26B702"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2990"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="529"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3A737A9013AE31342143AAC332FEB1D70166A3"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="475CE45464FC5C44EC1491CD403B214C11B264"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="84E0CECCD8B11684AA8882828679A4649A6238"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9DF148E8B9C34E949E39BB769715A2AAD5B239"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="794"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
@@ -852,7 +954,109 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2C443C73C2139424511282E223BA9D59E01A72"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1C2F7952D1F41C14E781A8601CF9C77B05EF91"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="12486F748194FB14E891ADBE158DFF48F524B1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1376"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1A18C20641A72C1401B18C5C1A90A56B754661"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BBCC80AD153C4144421923510F58B2602C731"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1454BFB5E1D645141091B73211A51887DA7C71"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -869,216 +1073,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1454BFB5E1D645141091B73211A51887DA7C71"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BBCC80AD153C4144421923510F58B2602C731"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1A18C20641A72C1401B18C5C1A90A56B754661"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1535"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="12486F748194FB14E891ADBE158DFF48F524B1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1376"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1E2A52455132D914AEE1AEF2144BD19AEA9CE1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="6218"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="556"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1C2F7952D1F41C14E781A8601CF9C77B05EF91"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2C443C73C2139424511282E223BA9D59E01A72"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="4710"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="6773"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="9DF148E8B9C34E949E39BB769715A2AAD5B239"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="794"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="84E0CECCD8B11684AA8882828679A4649A6238"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="767"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="475CE45464FC5C44EC1491CD403B214C11B264"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1217"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3A737A9013AE31342143AAC332FEB1D70166A3"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1429"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="22AE137DF231F5242212B9B62458710E26B702"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2990"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="529"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B9CFAB0817D4614E371BA261C76ECA0C6DA41"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B41DF30A103CB1433018E231B7416FB5ED861"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1112,7 +1112,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B41DF30A103CB1433018E231B7416FB5ED861"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B9CFAB0817D4614E371BA261C76ECA0C6DA41"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1367,11 +1367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="424022376"/>
-        <c:axId val="424027472"/>
+        <c:axId val="450229984"/>
+        <c:axId val="450226456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424022376"/>
+        <c:axId val="450229984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424027472"/>
+        <c:crossAx val="450226456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424027472"/>
+        <c:axId val="450226456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1472,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424022376"/>
+        <c:crossAx val="450229984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1738,11 +1738,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="424024336"/>
-        <c:axId val="424410080"/>
+        <c:axId val="450735912"/>
+        <c:axId val="450737872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424024336"/>
+        <c:axId val="450735912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424410080"/>
+        <c:crossAx val="450737872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1792,7 +1792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424410080"/>
+        <c:axId val="450737872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,7 +1843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424024336"/>
+        <c:crossAx val="450735912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2152,11 +2152,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="424410472"/>
-        <c:axId val="424409296"/>
+        <c:axId val="450739440"/>
+        <c:axId val="450736696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424410472"/>
+        <c:axId val="450739440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2198,7 +2198,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424409296"/>
+        <c:crossAx val="450736696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2206,7 +2206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424409296"/>
+        <c:axId val="450736696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424410472"/>
+        <c:crossAx val="450739440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4037,7 +4037,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4099,7 +4099,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4161,7 +4161,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4223,7 +4223,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4285,7 +4285,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4347,7 +4347,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4409,7 +4409,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4471,7 +4471,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4533,7 +4533,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4595,7 +4595,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4657,7 +4657,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4719,7 +4719,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4781,7 +4781,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4843,7 +4843,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4905,7 +4905,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38AB541D-4CF7-4DDA-B363-D444372BF1B1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38AB541D-4CF7-4DDA-B363-D444372BF1B1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5002,7 +5002,7 @@
                   <a14:compatExt spid="_x0000_s5121"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001140000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5064,7 +5064,7 @@
                   <a14:compatExt spid="_x0000_s5122"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002140000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5121,7 +5121,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5157,7 +5157,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5648,8 +5648,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BA84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,34 +5674,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:53" ht="26.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="E2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="I2" s="23" t="s">
         <v>51</v>
       </c>
@@ -5725,17 +5725,17 @@
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="38" t="s">
+      <c r="R2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="7"/>
-      <c r="V2" s="38" t="s">
+      <c r="V2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
       <c r="AM2" s="25" t="s">
         <v>70</v>
       </c>
@@ -5777,12 +5777,12 @@
       </c>
     </row>
     <row r="3" spans="1:53" ht="9.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="9"/>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
@@ -5793,13 +5793,13 @@
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -6532,12 +6532,12 @@
       </c>
     </row>
     <row r="19" spans="1:47" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -6602,10 +6602,10 @@
       </c>
     </row>
     <row r="21" spans="1:47" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="34"/>
+      <c r="G21" s="37"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
@@ -6633,8 +6633,8 @@
       </c>
     </row>
     <row r="22" spans="1:47" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
@@ -6662,8 +6662,8 @@
       </c>
     </row>
     <row r="23" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -6691,8 +6691,8 @@
       </c>
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
@@ -6720,8 +6720,8 @@
       </c>
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -6749,8 +6749,8 @@
       </c>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -6778,8 +6778,8 @@
       </c>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
@@ -6980,466 +6980,466 @@
       </c>
     </row>
     <row r="40" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
     </row>
     <row r="41" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
     </row>
     <row r="42" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="30"/>
     </row>
     <row r="43" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="30"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="30"/>
+      <c r="N43" s="30"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="30"/>
     </row>
     <row r="44" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="42"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="42"/>
-      <c r="N44" s="42"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="42"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="30"/>
+      <c r="M44" s="30"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="30"/>
     </row>
     <row r="45" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="42"/>
-      <c r="O45" s="42"/>
-      <c r="P45" s="42"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
+      <c r="P45" s="30"/>
     </row>
     <row r="46" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="42"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="42"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="30"/>
     </row>
     <row r="47" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="42"/>
-      <c r="N47" s="42"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="42"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
     </row>
     <row r="48" spans="9:47" x14ac:dyDescent="0.25">
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="42"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="42"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30"/>
+      <c r="N48" s="30"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="30"/>
     </row>
     <row r="49" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="42"/>
-      <c r="N49" s="42"/>
-      <c r="O49" s="42"/>
-      <c r="P49" s="42"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="30"/>
+      <c r="N49" s="30"/>
+      <c r="O49" s="30"/>
+      <c r="P49" s="30"/>
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="42"/>
-      <c r="L50" s="42"/>
-      <c r="M50" s="42"/>
-      <c r="N50" s="42"/>
-      <c r="O50" s="42"/>
-      <c r="P50" s="42"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
+      <c r="N50" s="30"/>
+      <c r="O50" s="30"/>
+      <c r="P50" s="30"/>
     </row>
     <row r="51" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="42"/>
-      <c r="L51" s="42"/>
-      <c r="M51" s="42"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="42"/>
-      <c r="P51" s="42"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
     </row>
     <row r="52" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I52" s="42"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="42"/>
-      <c r="N52" s="42"/>
-      <c r="O52" s="42"/>
-      <c r="P52" s="42"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="30"/>
+      <c r="K52" s="30"/>
+      <c r="L52" s="30"/>
+      <c r="M52" s="30"/>
+      <c r="N52" s="30"/>
+      <c r="O52" s="30"/>
+      <c r="P52" s="30"/>
     </row>
     <row r="53" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="42"/>
-      <c r="N53" s="42"/>
-      <c r="O53" s="42"/>
-      <c r="P53" s="42"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="30"/>
+      <c r="L53" s="30"/>
+      <c r="M53" s="30"/>
+      <c r="N53" s="30"/>
+      <c r="O53" s="30"/>
+      <c r="P53" s="30"/>
     </row>
     <row r="54" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="42"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="42"/>
-      <c r="N54" s="42"/>
-      <c r="O54" s="42"/>
-      <c r="P54" s="42"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="30"/>
+      <c r="K54" s="30"/>
+      <c r="L54" s="30"/>
+      <c r="M54" s="30"/>
+      <c r="N54" s="30"/>
+      <c r="O54" s="30"/>
+      <c r="P54" s="30"/>
     </row>
     <row r="55" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I55" s="42"/>
-      <c r="J55" s="42"/>
-      <c r="K55" s="42"/>
-      <c r="L55" s="42"/>
-      <c r="M55" s="42"/>
-      <c r="N55" s="42"/>
-      <c r="O55" s="42"/>
-      <c r="P55" s="42"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="30"/>
+      <c r="L55" s="30"/>
+      <c r="M55" s="30"/>
+      <c r="N55" s="30"/>
+      <c r="O55" s="30"/>
+      <c r="P55" s="30"/>
     </row>
     <row r="56" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I56" s="42"/>
-      <c r="J56" s="42"/>
-      <c r="K56" s="42"/>
-      <c r="L56" s="42"/>
-      <c r="M56" s="42"/>
-      <c r="N56" s="42"/>
-      <c r="O56" s="42"/>
-      <c r="P56" s="42"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
+      <c r="L56" s="30"/>
+      <c r="M56" s="30"/>
+      <c r="N56" s="30"/>
+      <c r="O56" s="30"/>
+      <c r="P56" s="30"/>
     </row>
     <row r="57" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I57" s="42"/>
-      <c r="J57" s="42"/>
-      <c r="K57" s="42"/>
-      <c r="L57" s="42"/>
-      <c r="M57" s="42"/>
-      <c r="N57" s="42"/>
-      <c r="O57" s="42"/>
-      <c r="P57" s="42"/>
+      <c r="I57" s="30"/>
+      <c r="J57" s="30"/>
+      <c r="K57" s="30"/>
+      <c r="L57" s="30"/>
+      <c r="M57" s="30"/>
+      <c r="N57" s="30"/>
+      <c r="O57" s="30"/>
+      <c r="P57" s="30"/>
     </row>
     <row r="58" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I58" s="42"/>
-      <c r="J58" s="42"/>
-      <c r="K58" s="42"/>
-      <c r="L58" s="42"/>
-      <c r="M58" s="42"/>
-      <c r="N58" s="42"/>
-      <c r="O58" s="42"/>
-      <c r="P58" s="42"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="30"/>
+      <c r="K58" s="30"/>
+      <c r="L58" s="30"/>
+      <c r="M58" s="30"/>
+      <c r="N58" s="30"/>
+      <c r="O58" s="30"/>
+      <c r="P58" s="30"/>
     </row>
     <row r="59" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="42"/>
-      <c r="M59" s="42"/>
-      <c r="N59" s="42"/>
-      <c r="O59" s="42"/>
-      <c r="P59" s="42"/>
+      <c r="I59" s="30"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="30"/>
+      <c r="L59" s="30"/>
+      <c r="M59" s="30"/>
+      <c r="N59" s="30"/>
+      <c r="O59" s="30"/>
+      <c r="P59" s="30"/>
     </row>
     <row r="60" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I60" s="42"/>
-      <c r="J60" s="42"/>
-      <c r="K60" s="42"/>
-      <c r="L60" s="42"/>
-      <c r="M60" s="42"/>
-      <c r="N60" s="42"/>
-      <c r="O60" s="42"/>
-      <c r="P60" s="42"/>
+      <c r="I60" s="30"/>
+      <c r="J60" s="30"/>
+      <c r="K60" s="30"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="30"/>
+      <c r="N60" s="30"/>
+      <c r="O60" s="30"/>
+      <c r="P60" s="30"/>
     </row>
     <row r="61" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I61" s="42"/>
-      <c r="J61" s="42"/>
-      <c r="K61" s="42"/>
-      <c r="L61" s="42"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="42"/>
-      <c r="O61" s="42"/>
-      <c r="P61" s="42"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30"/>
+      <c r="L61" s="30"/>
+      <c r="M61" s="30"/>
+      <c r="N61" s="30"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="30"/>
     </row>
     <row r="62" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I62" s="42"/>
-      <c r="J62" s="42"/>
-      <c r="K62" s="42"/>
-      <c r="L62" s="42"/>
-      <c r="M62" s="42"/>
-      <c r="N62" s="42"/>
-      <c r="O62" s="42"/>
-      <c r="P62" s="42"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="30"/>
+      <c r="L62" s="30"/>
+      <c r="M62" s="30"/>
+      <c r="N62" s="30"/>
+      <c r="O62" s="30"/>
+      <c r="P62" s="30"/>
     </row>
     <row r="63" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I63" s="42"/>
-      <c r="J63" s="42"/>
-      <c r="K63" s="42"/>
-      <c r="L63" s="42"/>
-      <c r="M63" s="42"/>
-      <c r="N63" s="42"/>
-      <c r="O63" s="42"/>
-      <c r="P63" s="42"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="30"/>
+      <c r="L63" s="30"/>
+      <c r="M63" s="30"/>
+      <c r="N63" s="30"/>
+      <c r="O63" s="30"/>
+      <c r="P63" s="30"/>
     </row>
     <row r="64" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I64" s="42"/>
-      <c r="J64" s="42"/>
-      <c r="K64" s="42"/>
-      <c r="L64" s="42"/>
-      <c r="M64" s="42"/>
-      <c r="N64" s="42"/>
-      <c r="O64" s="42"/>
-      <c r="P64" s="42"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="30"/>
+      <c r="K64" s="30"/>
+      <c r="L64" s="30"/>
+      <c r="M64" s="30"/>
+      <c r="N64" s="30"/>
+      <c r="O64" s="30"/>
+      <c r="P64" s="30"/>
     </row>
     <row r="65" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I65" s="42"/>
-      <c r="J65" s="42"/>
-      <c r="K65" s="42"/>
-      <c r="L65" s="42"/>
-      <c r="M65" s="42"/>
-      <c r="N65" s="42"/>
-      <c r="O65" s="42"/>
-      <c r="P65" s="42"/>
+      <c r="I65" s="30"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="30"/>
+      <c r="L65" s="30"/>
+      <c r="M65" s="30"/>
+      <c r="N65" s="30"/>
+      <c r="O65" s="30"/>
+      <c r="P65" s="30"/>
     </row>
     <row r="66" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I66" s="42"/>
-      <c r="J66" s="42"/>
-      <c r="K66" s="42"/>
-      <c r="L66" s="42"/>
-      <c r="M66" s="42"/>
-      <c r="N66" s="42"/>
-      <c r="O66" s="42"/>
-      <c r="P66" s="42"/>
+      <c r="I66" s="30"/>
+      <c r="J66" s="30"/>
+      <c r="K66" s="30"/>
+      <c r="L66" s="30"/>
+      <c r="M66" s="30"/>
+      <c r="N66" s="30"/>
+      <c r="O66" s="30"/>
+      <c r="P66" s="30"/>
     </row>
     <row r="67" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I67" s="42"/>
-      <c r="J67" s="42"/>
-      <c r="K67" s="42"/>
-      <c r="L67" s="42"/>
-      <c r="M67" s="42"/>
-      <c r="N67" s="42"/>
-      <c r="O67" s="42"/>
-      <c r="P67" s="42"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="30"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="30"/>
+      <c r="N67" s="30"/>
+      <c r="O67" s="30"/>
+      <c r="P67" s="30"/>
     </row>
     <row r="68" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I68" s="42"/>
-      <c r="J68" s="42"/>
-      <c r="K68" s="42"/>
-      <c r="L68" s="42"/>
-      <c r="M68" s="42"/>
-      <c r="N68" s="42"/>
-      <c r="O68" s="42"/>
-      <c r="P68" s="42"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
+      <c r="N68" s="30"/>
+      <c r="O68" s="30"/>
+      <c r="P68" s="30"/>
     </row>
     <row r="69" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I69" s="42"/>
-      <c r="J69" s="42"/>
-      <c r="K69" s="42"/>
-      <c r="L69" s="42"/>
-      <c r="M69" s="42"/>
-      <c r="N69" s="42"/>
-      <c r="O69" s="42"/>
-      <c r="P69" s="42"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="30"/>
+      <c r="N69" s="30"/>
+      <c r="O69" s="30"/>
+      <c r="P69" s="30"/>
     </row>
     <row r="70" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I70" s="42"/>
-      <c r="J70" s="42"/>
-      <c r="K70" s="42"/>
-      <c r="L70" s="42"/>
-      <c r="M70" s="42"/>
-      <c r="N70" s="42"/>
-      <c r="O70" s="42"/>
-      <c r="P70" s="42"/>
+      <c r="I70" s="30"/>
+      <c r="J70" s="30"/>
+      <c r="K70" s="30"/>
+      <c r="L70" s="30"/>
+      <c r="M70" s="30"/>
+      <c r="N70" s="30"/>
+      <c r="O70" s="30"/>
+      <c r="P70" s="30"/>
     </row>
     <row r="71" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I71" s="42"/>
-      <c r="J71" s="42"/>
-      <c r="K71" s="42"/>
-      <c r="L71" s="42"/>
-      <c r="M71" s="42"/>
-      <c r="N71" s="42"/>
-      <c r="O71" s="42"/>
-      <c r="P71" s="42"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="30"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="30"/>
+      <c r="M71" s="30"/>
+      <c r="N71" s="30"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="30"/>
     </row>
     <row r="72" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I72" s="42"/>
-      <c r="J72" s="42"/>
-      <c r="K72" s="42"/>
-      <c r="L72" s="42"/>
-      <c r="M72" s="42"/>
-      <c r="N72" s="42"/>
-      <c r="O72" s="42"/>
-      <c r="P72" s="42"/>
+      <c r="I72" s="30"/>
+      <c r="J72" s="30"/>
+      <c r="K72" s="30"/>
+      <c r="L72" s="30"/>
+      <c r="M72" s="30"/>
+      <c r="N72" s="30"/>
+      <c r="O72" s="30"/>
+      <c r="P72" s="30"/>
     </row>
     <row r="73" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I73" s="42"/>
-      <c r="J73" s="42"/>
-      <c r="K73" s="42"/>
-      <c r="L73" s="42"/>
-      <c r="M73" s="42"/>
-      <c r="N73" s="42"/>
-      <c r="O73" s="42"/>
-      <c r="P73" s="42"/>
+      <c r="I73" s="30"/>
+      <c r="J73" s="30"/>
+      <c r="K73" s="30"/>
+      <c r="L73" s="30"/>
+      <c r="M73" s="30"/>
+      <c r="N73" s="30"/>
+      <c r="O73" s="30"/>
+      <c r="P73" s="30"/>
     </row>
     <row r="74" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I74" s="42"/>
-      <c r="J74" s="42"/>
-      <c r="K74" s="42"/>
-      <c r="L74" s="42"/>
-      <c r="M74" s="42"/>
-      <c r="N74" s="42"/>
-      <c r="O74" s="42"/>
-      <c r="P74" s="42"/>
+      <c r="I74" s="30"/>
+      <c r="J74" s="30"/>
+      <c r="K74" s="30"/>
+      <c r="L74" s="30"/>
+      <c r="M74" s="30"/>
+      <c r="N74" s="30"/>
+      <c r="O74" s="30"/>
+      <c r="P74" s="30"/>
     </row>
     <row r="75" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I75" s="42"/>
-      <c r="J75" s="42"/>
-      <c r="K75" s="42"/>
-      <c r="L75" s="42"/>
-      <c r="M75" s="42"/>
-      <c r="N75" s="42"/>
-      <c r="O75" s="42"/>
-      <c r="P75" s="42"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+      <c r="L75" s="30"/>
+      <c r="M75" s="30"/>
+      <c r="N75" s="30"/>
+      <c r="O75" s="30"/>
+      <c r="P75" s="30"/>
     </row>
     <row r="76" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I76" s="42"/>
-      <c r="J76" s="42"/>
-      <c r="K76" s="42"/>
-      <c r="L76" s="42"/>
-      <c r="M76" s="42"/>
-      <c r="N76" s="42"/>
-      <c r="O76" s="42"/>
-      <c r="P76" s="42"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="30"/>
+      <c r="K76" s="30"/>
+      <c r="L76" s="30"/>
+      <c r="M76" s="30"/>
+      <c r="N76" s="30"/>
+      <c r="O76" s="30"/>
+      <c r="P76" s="30"/>
     </row>
     <row r="77" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I77" s="42"/>
-      <c r="J77" s="42"/>
-      <c r="K77" s="42"/>
-      <c r="L77" s="42"/>
-      <c r="M77" s="42"/>
-      <c r="N77" s="42"/>
-      <c r="O77" s="42"/>
-      <c r="P77" s="42"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="30"/>
+      <c r="K77" s="30"/>
+      <c r="L77" s="30"/>
+      <c r="M77" s="30"/>
+      <c r="N77" s="30"/>
+      <c r="O77" s="30"/>
+      <c r="P77" s="30"/>
     </row>
     <row r="78" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I78" s="42"/>
-      <c r="J78" s="42"/>
-      <c r="K78" s="42"/>
-      <c r="L78" s="42"/>
-      <c r="M78" s="42"/>
-      <c r="N78" s="42"/>
-      <c r="O78" s="42"/>
-      <c r="P78" s="42"/>
+      <c r="I78" s="30"/>
+      <c r="J78" s="30"/>
+      <c r="K78" s="30"/>
+      <c r="L78" s="30"/>
+      <c r="M78" s="30"/>
+      <c r="N78" s="30"/>
+      <c r="O78" s="30"/>
+      <c r="P78" s="30"/>
     </row>
     <row r="79" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I79" s="42"/>
-      <c r="J79" s="42"/>
-      <c r="K79" s="42"/>
-      <c r="L79" s="42"/>
-      <c r="M79" s="42"/>
-      <c r="N79" s="42"/>
-      <c r="O79" s="42"/>
-      <c r="P79" s="42"/>
+      <c r="I79" s="30"/>
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+      <c r="L79" s="30"/>
+      <c r="M79" s="30"/>
+      <c r="N79" s="30"/>
+      <c r="O79" s="30"/>
+      <c r="P79" s="30"/>
     </row>
     <row r="80" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I80" s="42"/>
-      <c r="J80" s="42"/>
-      <c r="K80" s="42"/>
-      <c r="L80" s="42"/>
-      <c r="M80" s="42"/>
-      <c r="N80" s="42"/>
-      <c r="O80" s="42"/>
-      <c r="P80" s="42"/>
+      <c r="I80" s="30"/>
+      <c r="J80" s="30"/>
+      <c r="K80" s="30"/>
+      <c r="L80" s="30"/>
+      <c r="M80" s="30"/>
+      <c r="N80" s="30"/>
+      <c r="O80" s="30"/>
+      <c r="P80" s="30"/>
     </row>
     <row r="81" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I81" s="42"/>
-      <c r="J81" s="42"/>
-      <c r="K81" s="42"/>
-      <c r="L81" s="42"/>
-      <c r="M81" s="42"/>
-      <c r="N81" s="42"/>
-      <c r="O81" s="42"/>
-      <c r="P81" s="42"/>
+      <c r="I81" s="30"/>
+      <c r="J81" s="30"/>
+      <c r="K81" s="30"/>
+      <c r="L81" s="30"/>
+      <c r="M81" s="30"/>
+      <c r="N81" s="30"/>
+      <c r="O81" s="30"/>
+      <c r="P81" s="30"/>
     </row>
     <row r="82" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I82" s="42"/>
-      <c r="J82" s="42"/>
-      <c r="K82" s="42"/>
-      <c r="L82" s="42"/>
-      <c r="M82" s="42"/>
-      <c r="N82" s="42"/>
-      <c r="O82" s="42"/>
-      <c r="P82" s="42"/>
+      <c r="I82" s="30"/>
+      <c r="J82" s="30"/>
+      <c r="K82" s="30"/>
+      <c r="L82" s="30"/>
+      <c r="M82" s="30"/>
+      <c r="N82" s="30"/>
+      <c r="O82" s="30"/>
+      <c r="P82" s="30"/>
     </row>
     <row r="83" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I83" s="42"/>
-      <c r="J83" s="42"/>
-      <c r="K83" s="42"/>
-      <c r="L83" s="42"/>
-      <c r="M83" s="42"/>
-      <c r="N83" s="42"/>
-      <c r="O83" s="42"/>
-      <c r="P83" s="42"/>
+      <c r="I83" s="30"/>
+      <c r="J83" s="30"/>
+      <c r="K83" s="30"/>
+      <c r="L83" s="30"/>
+      <c r="M83" s="30"/>
+      <c r="N83" s="30"/>
+      <c r="O83" s="30"/>
+      <c r="P83" s="30"/>
     </row>
     <row r="84" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I84" s="42"/>
-      <c r="J84" s="42"/>
-      <c r="K84" s="42"/>
-      <c r="L84" s="42"/>
-      <c r="M84" s="42"/>
-      <c r="N84" s="42"/>
-      <c r="O84" s="42"/>
-      <c r="P84" s="42"/>
+      <c r="I84" s="30"/>
+      <c r="J84" s="30"/>
+      <c r="K84" s="30"/>
+      <c r="L84" s="30"/>
+      <c r="M84" s="30"/>
+      <c r="N84" s="30"/>
+      <c r="O84" s="30"/>
+      <c r="P84" s="30"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="8">
+    <mergeCell ref="F21:G27"/>
+    <mergeCell ref="A19:D19"/>
     <mergeCell ref="R2:T3"/>
     <mergeCell ref="V2:X3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="H1:M1"/>
-    <mergeCell ref="F21:G27"/>
-    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7448,19 +7448,169 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper15">
+        <control shapeId="1041" r:id="rId4" name="_ActiveXWrapper14">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
-                <xdr:row>38</xdr:row>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>504825</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1041" r:id="rId4" name="_ActiveXWrapper14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1040" r:id="rId6" name="_ActiveXWrapper13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1040" r:id="rId6" name="_ActiveXWrapper13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId8" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId8" name="_ActiveXWrapper12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId10" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId10" name="_ActiveXWrapper11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1037" r:id="rId12" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>514350</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId12" name="_ActiveXWrapper10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>17</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>60</xdr:row>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId16" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -7468,157 +7618,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId6" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId6" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId8" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId8" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId10" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId12" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>542925</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId12" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId14" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>200025</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>590550</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId14" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId16" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId16" name="_ActiveXWrapper1"/>
+        <control shapeId="1035" r:id="rId16" name="_ActiveXWrapper8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7648,19 +7648,169 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId20" name="_ActiveXWrapper8">
+        <control shapeId="1025" r:id="rId20" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId21">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId20" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId22" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>590550</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId22" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId24" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>542925</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId24" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId26" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId27">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId26" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId28" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId29">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>209550</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId28" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1033" r:id="rId30" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId31">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId30" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1042" r:id="rId32" name="_ActiveXWrapper15">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId33">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>17</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>60</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -7668,164 +7818,14 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1035" r:id="rId20" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId22" name="_ActiveXWrapper9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId22" name="_ActiveXWrapper9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId24" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1037" r:id="rId24" name="_ActiveXWrapper10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId26" name="_ActiveXWrapper11">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1038" r:id="rId26" name="_ActiveXWrapper11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId28" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId29">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1039" r:id="rId28" name="_ActiveXWrapper12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId30" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId31">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>104775</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1040" r:id="rId30" name="_ActiveXWrapper13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId32" name="_ActiveXWrapper14">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>504825</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1041" r:id="rId32" name="_ActiveXWrapper14"/>
+        <control shapeId="1042" r:id="rId32" name="_ActiveXWrapper15"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
   <tableParts count="3">
-    <tablePart r:id="rId33"/>
     <tablePart r:id="rId34"/>
     <tablePart r:id="rId35"/>
+    <tablePart r:id="rId36"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7876,8 +7876,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="5121" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="5122" r:id="rId4" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>371475</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="5122" r:id="rId4" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="5121" r:id="rId6" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -7896,32 +7921,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="5121" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="5122" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>371475</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="5122" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="5121" r:id="rId6" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7947,27 +7947,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="Q1" s="41" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="Q1" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>